<commit_message>
Updating ice hockey results
</commit_message>
<xml_diff>
--- a/data-raw/ice_hockey_championships.xlsx
+++ b/data-raw/ice_hockey_championships.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="rankings" sheetId="1" state="visible" r:id="rId2"/>
@@ -203,13 +203,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Y26"/>
+  <dimension ref="A1:Y27"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K26" activeCellId="0" sqref="K26"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A47" activeCellId="0" sqref="A47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.54"/>
   </cols>
@@ -1565,6 +1565,59 @@
         <v>6</v>
       </c>
       <c r="Y26" s="0" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="1" t="n">
+        <v>2023</v>
+      </c>
+      <c r="B27" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="D27" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E27" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="F27" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="G27" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="H27" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="I27" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="J27" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="L27" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="O27" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="Q27" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="R27" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="U27" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="V27" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="W27" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="Y27" s="0" t="n">
         <v>4</v>
       </c>
     </row>
@@ -1584,13 +1637,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Y25"/>
+  <dimension ref="A1:Y27"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C32" activeCellId="0" sqref="C32"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C41" activeCellId="0" sqref="C41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.54"/>
   </cols>
@@ -3445,6 +3498,160 @@
         <v>0</v>
       </c>
       <c r="Y25" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="1" t="n">
+        <v>2022</v>
+      </c>
+      <c r="B26" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C26" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D26" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E26" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F26" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G26" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H26" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I26" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="J26" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K26" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="L26" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="M26" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="N26" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O26" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P26" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q26" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="R26" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S26" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="T26" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="U26" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="V26" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="W26" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="X26" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y26" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="1" t="n">
+        <v>2023</v>
+      </c>
+      <c r="B27" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C27" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D27" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E27" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F27" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G27" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H27" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I27" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="J27" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K27" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="L27" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="M27" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="N27" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O27" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P27" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q27" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="R27" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S27" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="T27" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="U27" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="V27" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="W27" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="X27" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y27" s="0" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Corrected 2018 host country in the ice_hockey_championships dataset
</commit_message>
<xml_diff>
--- a/data-raw/ice_hockey_championships.xlsx
+++ b/data-raw/ice_hockey_championships.xlsx
@@ -209,7 +209,7 @@
       <selection pane="topLeft" activeCell="A47" activeCellId="0" sqref="A47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.54"/>
   </cols>
@@ -1640,10 +1640,10 @@
   <dimension ref="A1:Y27"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C41" activeCellId="0" sqref="C41"/>
+      <selection pane="topLeft" activeCell="H22" activeCellId="0" sqref="H22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.54"/>
   </cols>
@@ -3288,7 +3288,7 @@
         <v>0</v>
       </c>
       <c r="H22" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I22" s="0" t="n">
         <v>0</v>

</xml_diff>